<commit_message>
Revert "Merge branch 'main' of https://github.com/RIT-SWEN-261-02/team-project-2215-section-02-2215-swen-261-02-c-straightflush"
This reverts commit 4c7f001840088253132d190e0f5542af2ceb9bf2, reversing
changes made to 71927331efb4cd0eb0655fb39f1b3aaf705f5417.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\rtyocum\code\rit\swen-261\team-project\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DB2909-7A15-4FB3-B94D-104EF3186DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76859C1D-AFC3-47A2-B16B-1D78C8ECEA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Instructions</t>
   </si>
@@ -64,6 +64,9 @@
     <t>Given that I am on the Products page when there are no products in the inventory I see a message indicating that that there are no products available.</t>
   </si>
   <si>
+    <t>Given that I am on the products page when there are products in the inventory then I see each product and short description.</t>
+  </si>
+  <si>
     <t>Given that I am on the products page when there are products in the inventory then I see a means to add each product to my shopping cart.</t>
   </si>
   <si>
@@ -76,93 +79,6 @@
   </si>
   <si>
     <t>2215-swen-261-02-c-straightflush</t>
-  </si>
-  <si>
-    <t>As a buyer I want to see a single product so that I can see a product's details.</t>
-  </si>
-  <si>
-    <t>Given that I am on the e-store site when I am on the Products page I can navigate to an individual product page</t>
-  </si>
-  <si>
-    <t>Given that I am not on the Products page when I choose the Product I go to the single product page</t>
-  </si>
-  <si>
-    <t>Given that I go to a products page of a product that does not exist, I am shown a 404 to show that the product does not exist</t>
-  </si>
-  <si>
-    <t>Given that I am on the products page when there are products in the inventory then I see each product and the price</t>
-  </si>
-  <si>
-    <t>Given that I am on the product page when the are product is in the inventory then I see a means to add the product to my shopping cart.</t>
-  </si>
-  <si>
-    <t>Given that I am on the product page when the product is in the inventory then I see each product and short description.</t>
-  </si>
-  <si>
-    <t>Given that I am on the e-store site when I am not on the Login page them I must see a means to navigate to the Login page</t>
-  </si>
-  <si>
-    <t>Given that I am not on the Products page when I choose the Login button I go to the login page</t>
-  </si>
-  <si>
-    <t>As a buyer I want to log in to save my cart</t>
-  </si>
-  <si>
-    <t>As an owner I want to log in</t>
-  </si>
-  <si>
-    <t>As an owner I want to see a single product so that I can see a product's details.</t>
-  </si>
-  <si>
-    <t>As an owner I want to edit a single product so that I can change a product's details.</t>
-  </si>
-  <si>
-    <t>Given that I am on the product page when the are product is in the inventory then I see a means edit a products name, description, price, and quantity</t>
-  </si>
-  <si>
-    <t>Given that I am on the product page when the are product is in the inventory then I see a means to delete a product</t>
-  </si>
-  <si>
-    <t>Given that I am on the e-store site when I am not on the Cart page them I must see a means to navigate to the Cart page</t>
-  </si>
-  <si>
-    <t>Given that I am not on the Login page when I choose the Login button I go to the login page</t>
-  </si>
-  <si>
-    <t>Given that I refresh the page I am still logged in</t>
-  </si>
-  <si>
-    <t>Given that I am not on the Cart page when I choose the Cart button I go to the Cart page</t>
-  </si>
-  <si>
-    <t>Given that I am on the cart page I can see the items in my cart</t>
-  </si>
-  <si>
-    <t>Given that I am on the cart page I can delete items from my cart</t>
-  </si>
-  <si>
-    <t>Given that I am on the cart page I can update the quantity of items in my cart</t>
-  </si>
-  <si>
-    <t>As an buyer I want to add and delete items from my cart so that I can checkout with those items</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>RY; 3/14/22</t>
-  </si>
-  <si>
-    <t>Given that I am on the products page, when I enter a search parameter and click Go, it returns the search results</t>
-  </si>
-  <si>
-    <t>RT; 3/14/22</t>
-  </si>
-  <si>
-    <t>NA; 3/14/22</t>
-  </si>
-  <si>
-    <t>CR; 3/14/22</t>
   </si>
 </sst>
 </file>
@@ -224,17 +140,17 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -260,12 +176,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -646,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -661,7 +571,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -669,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -690,11 +600,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F585"/>
+  <dimension ref="A1:F587"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E29" sqref="E29"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -735,12 +645,7 @@
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="C2" s="8"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
@@ -748,12 +653,7 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="C3" s="8"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -761,442 +661,192 @@
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="C5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="C6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="42" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="8"/>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="8"/>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="31.8" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
-      </c>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="8"/>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="31.8" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="8"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="42" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="8"/>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="8"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="8"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" ht="42" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="8"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="8"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="8"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="8"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="8"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>42</v>
-      </c>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="8"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" ht="42" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>30</v>
-      </c>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" s="8"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="2" t="s">
-        <v>33</v>
-      </c>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C31" s="8"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="2" t="s">
-        <v>34</v>
-      </c>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" s="8"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
-        <v>35</v>
-      </c>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="8"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12" t="s">
-        <v>36</v>
-      </c>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34" s="8"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35" s="8"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C36" s="8"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C37" s="8"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" s="8"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C39" s="8"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C40" s="8"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C41" s="8"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C42" s="8"/>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C43" s="8"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C44" s="8"/>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C45" s="8"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C46" s="8"/>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C47" s="8"/>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C48" s="8"/>
       <c r="E48" s="8"/>
     </row>
@@ -3348,9 +2998,17 @@
       <c r="C585" s="8"/>
       <c r="E585" s="8"/>
     </row>
+    <row r="586" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C586" s="8"/>
+      <c r="E586" s="8"/>
+    </row>
+    <row r="587" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C587" s="8"/>
+      <c r="E587" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C2:C585 E2:E585">
+  <conditionalFormatting sqref="C2:C587 E2:E587">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3358,7 +3016,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D585 F2:F585">
+  <conditionalFormatting sqref="D2:D587 F2:F587">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -3367,12 +3025,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C585 E2:E585" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C587 E2:E587" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>